<commit_message>
battle auto turn & bug fix
</commit_message>
<xml_diff>
--- a/Data/EnemyDefine.xlsx
+++ b/Data/EnemyDefine.xlsx
@@ -27,12 +27,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>ID</t>
   </si>
   <si>
     <t>CID</t>
+  </si>
+  <si>
+    <t>aiType</t>
   </si>
   <si>
     <t>equip1.id</t>
@@ -1240,32 +1243,32 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="4"/>
   <cols>
-    <col min="4" max="4" width="15.0480769230769" customWidth="1"/>
-    <col min="5" max="5" width="14.4134615384615" customWidth="1"/>
-    <col min="6" max="6" width="13.4615384615385" customWidth="1"/>
-    <col min="8" max="8" width="15.0576923076923" customWidth="1"/>
-    <col min="9" max="9" width="14.7403846153846" customWidth="1"/>
-    <col min="10" max="10" width="14.9038461538462" customWidth="1"/>
-    <col min="12" max="12" width="14.5769230769231" customWidth="1"/>
-    <col min="13" max="13" width="14.9038461538462" customWidth="1"/>
-    <col min="14" max="14" width="15.8557692307692" customWidth="1"/>
-    <col min="16" max="16" width="15.5384615384615" customWidth="1"/>
-    <col min="17" max="17" width="14.7403846153846" customWidth="1"/>
-    <col min="18" max="18" width="14.5769230769231" customWidth="1"/>
-    <col min="20" max="20" width="14.5865384615385" customWidth="1"/>
-    <col min="21" max="21" width="15.0576923076923" customWidth="1"/>
-    <col min="22" max="22" width="14.0961538461538" customWidth="1"/>
+    <col min="5" max="5" width="15.0480769230769" customWidth="1"/>
+    <col min="6" max="6" width="14.4134615384615" customWidth="1"/>
+    <col min="7" max="7" width="13.4615384615385" customWidth="1"/>
+    <col min="9" max="9" width="15.0576923076923" customWidth="1"/>
+    <col min="10" max="10" width="14.7403846153846" customWidth="1"/>
+    <col min="11" max="11" width="14.9038461538462" customWidth="1"/>
+    <col min="13" max="13" width="14.5769230769231" customWidth="1"/>
+    <col min="14" max="14" width="14.9038461538462" customWidth="1"/>
+    <col min="15" max="15" width="15.8557692307692" customWidth="1"/>
+    <col min="17" max="17" width="15.5384615384615" customWidth="1"/>
+    <col min="18" max="18" width="14.7403846153846" customWidth="1"/>
+    <col min="19" max="19" width="14.5769230769231" customWidth="1"/>
+    <col min="21" max="21" width="14.5865384615385" customWidth="1"/>
+    <col min="22" max="22" width="15.0576923076923" customWidth="1"/>
+    <col min="23" max="23" width="14.0961538461538" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1332,8 +1335,11 @@
       <c r="V1" t="s">
         <v>21</v>
       </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1341,7 +1347,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1353,44 +1359,125 @@
         <v>0</v>
       </c>
       <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>1</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
       <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
         <v>1</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
       <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
         <v>2</v>
       </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
       <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
         <v>2</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:1">

</xml_diff>

<commit_message>
battle support enermy logic
</commit_message>
<xml_diff>
--- a/Data/EnemyDefine.xlsx
+++ b/Data/EnemyDefine.xlsx
@@ -1243,13 +1243,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="6"/>
   <cols>
     <col min="5" max="5" width="15.0480769230769" customWidth="1"/>
     <col min="6" max="6" width="14.4134615384615" customWidth="1"/>
@@ -1344,7 +1344,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1391,7 +1391,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1438,7 +1438,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1480,8 +1480,146 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="1"/>
+    <row r="5" spans="1:15">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>103</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>104</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>105</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>